<commit_message>
fixed issue with total price
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshuawolfson/Documents/Coding/CableChecker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0045E2-903E-E545-B71C-504777D14E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63ECCAC1-AEBE-9748-A73E-0CB7FC21C970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-12060" windowWidth="38400" windowHeight="23380" xr2:uid="{E48B5B42-38F6-7245-A75D-5DA71F556FEC}"/>
   </bookViews>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="59">
   <si>
     <t>Part</t>
   </si>
@@ -255,6 +255,9 @@
   </si>
   <si>
     <t>M1.6x12</t>
+  </si>
+  <si>
+    <t>PCB Assembly (for ES8388)</t>
   </si>
 </sst>
 </file>
@@ -1042,18 +1045,18 @@
     <v>Powered by Refinitiv</v>
     <v>1.6906000000000001</v>
     <v>1.4400999999999999</v>
-    <v>3.2000000000000002E-3</v>
-    <v>2.1060000000000002E-3</v>
+    <v>2.8E-3</v>
+    <v>1.843E-3</v>
     <v>AUD</v>
     <v>USD</v>
     <v>1.5253000000000001</v>
     <v>Currency Pair</v>
-    <v>45852.318287037036</v>
+    <v>45852.410069444442</v>
     <v>1.5181</v>
     <v>US Dollar/Australian Dollar FX Cross Rate</v>
     <v>1.5210999999999999</v>
     <v>1.5193000000000001</v>
-    <v>1.5225</v>
+    <v>1.5221</v>
     <v>USDAUD</v>
     <v>USD/AUD</v>
   </rv>
@@ -1074,18 +1077,18 @@
     <v>Powered by Refinitiv</v>
     <v>0.69420000000000004</v>
     <v>0.59119999999999995</v>
-    <v>-1.4E-3</v>
-    <v>-2.1279999999999997E-3</v>
+    <v>-1.1999999999999999E-3</v>
+    <v>-1.8240000000000001E-3</v>
     <v>USD</v>
     <v>AUD</v>
     <v>0.65869999999999995</v>
     <v>Currency Pair</v>
-    <v>45852.318287037036</v>
+    <v>45852.410069444442</v>
     <v>0.65559999999999996</v>
     <v>Australian Dollar/US Dollar FX Spot Rate</v>
     <v>0.6573</v>
     <v>0.65780000000000005</v>
-    <v>0.65639999999999998</v>
+    <v>0.65659999999999996</v>
     <v>AUDUSD</v>
     <v>AUD/USD</v>
   </rv>
@@ -1289,7 +1292,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F0D4220D-0A52-C34C-ACF8-42D2B19FEE5D}" name="Table1" displayName="Table1" ref="A1:K15" totalsRowCount="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F0D4220D-0A52-C34C-ACF8-42D2B19FEE5D}" name="Table1" displayName="Table1" ref="A1:K16" totalsRowCount="1">
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{E0204AEA-A418-7044-8059-FB3046E9F3CD}" name="Part" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{F873D4A1-7423-AF48-92FE-29E3B36ABD22}" name="SKU"/>
@@ -1630,10 +1633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BCCD5C7-319F-6741-AF08-94CC8C732899}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1715,7 +1718,7 @@
       </c>
       <c r="I2" s="5">
         <f ca="1">IF(Table1[[#This Row],[Price (AUD)]],SUM(Table1[[#This Row],[Shipping (AUD)]],Table1[[#This Row],[Price (AUD)]]),SUM(Table1[[#This Row],[Price (USD)]:[Shipping (USD)]])*Exchange!$B$2)</f>
-        <v>18.041625</v>
+        <v>18.036884999999998</v>
       </c>
       <c r="J2" s="5">
         <f>IF(Table1[[#This Row],[Price (USD)]],SUM(Table1[[#This Row],[Price (USD)]:[Shipping (USD)]]),SUM(Table1[[#This Row],[Shipping (AUD)]],Table1[[#This Row],[Price (AUD)]])*Exchange!$B$3)</f>
@@ -1752,7 +1755,7 @@
       </c>
       <c r="I3" s="5">
         <f ca="1">IF(Table1[[#This Row],[Price (AUD)]],SUM(Table1[[#This Row],[Shipping (AUD)]],Table1[[#This Row],[Price (AUD)]]),SUM(Table1[[#This Row],[Price (USD)]:[Shipping (USD)]])*Exchange!$B$2)</f>
-        <v>1.5681750000000001</v>
+        <v>1.567763</v>
       </c>
       <c r="J3" s="5">
         <f>IF(Table1[[#This Row],[Price (USD)]],SUM(Table1[[#This Row],[Price (USD)]:[Shipping (USD)]]),SUM(Table1[[#This Row],[Shipping (AUD)]],Table1[[#This Row],[Price (AUD)]])*Exchange!$B$3)</f>
@@ -1789,7 +1792,7 @@
       </c>
       <c r="I4" s="5">
         <f ca="1">IF(Table1[[#This Row],[Price (AUD)]],SUM(Table1[[#This Row],[Shipping (AUD)]],Table1[[#This Row],[Price (AUD)]]),SUM(Table1[[#This Row],[Price (USD)]:[Shipping (USD)]])*Exchange!$B$2)</f>
-        <v>2.3903250000000003</v>
+        <v>2.389697</v>
       </c>
       <c r="J4" s="5">
         <f>IF(Table1[[#This Row],[Price (USD)]],SUM(Table1[[#This Row],[Price (USD)]:[Shipping (USD)]]),SUM(Table1[[#This Row],[Shipping (AUD)]],Table1[[#This Row],[Price (AUD)]])*Exchange!$B$3)</f>
@@ -1826,7 +1829,7 @@
       </c>
       <c r="I5" s="5">
         <f ca="1">IF(Table1[[#This Row],[Price (AUD)]],SUM(Table1[[#This Row],[Shipping (AUD)]],Table1[[#This Row],[Price (AUD)]]),SUM(Table1[[#This Row],[Price (USD)]:[Shipping (USD)]])*Exchange!$B$2)</f>
-        <v>2.1771749999999996</v>
+        <v>2.1766030000000001</v>
       </c>
       <c r="J5" s="5">
         <f>IF(Table1[[#This Row],[Price (USD)]],SUM(Table1[[#This Row],[Price (USD)]:[Shipping (USD)]]),SUM(Table1[[#This Row],[Shipping (AUD)]],Table1[[#This Row],[Price (AUD)]])*Exchange!$B$3)</f>
@@ -1863,7 +1866,7 @@
       </c>
       <c r="I6" s="5">
         <f ca="1">IF(Table1[[#This Row],[Price (AUD)]],SUM(Table1[[#This Row],[Shipping (AUD)]],Table1[[#This Row],[Price (AUD)]]),SUM(Table1[[#This Row],[Price (USD)]:[Shipping (USD)]])*Exchange!$B$2)</f>
-        <v>1.7356499999999999</v>
+        <v>1.7351939999999999</v>
       </c>
       <c r="J6" s="5">
         <f>IF(Table1[[#This Row],[Price (USD)]],SUM(Table1[[#This Row],[Price (USD)]:[Shipping (USD)]]),SUM(Table1[[#This Row],[Shipping (AUD)]],Table1[[#This Row],[Price (AUD)]])*Exchange!$B$3)</f>
@@ -1900,7 +1903,7 @@
       </c>
       <c r="I7" s="5">
         <f ca="1">IF(Table1[[#This Row],[Price (AUD)]],SUM(Table1[[#This Row],[Shipping (AUD)]],Table1[[#This Row],[Price (AUD)]]),SUM(Table1[[#This Row],[Price (USD)]:[Shipping (USD)]])*Exchange!$B$2)</f>
-        <v>1.00485</v>
+        <v>1.004586</v>
       </c>
       <c r="J7" s="5">
         <f>IF(Table1[[#This Row],[Price (USD)]],SUM(Table1[[#This Row],[Price (USD)]:[Shipping (USD)]]),SUM(Table1[[#This Row],[Shipping (AUD)]],Table1[[#This Row],[Price (AUD)]])*Exchange!$B$3)</f>
@@ -1941,7 +1944,7 @@
       </c>
       <c r="J8" s="5">
         <f ca="1">IF(Table1[[#This Row],[Price (USD)]],SUM(Table1[[#This Row],[Price (USD)]:[Shipping (USD)]]),SUM(Table1[[#This Row],[Shipping (AUD)]],Table1[[#This Row],[Price (AUD)]])*Exchange!$B$3)</f>
-        <v>6.1045199999999999</v>
+        <v>6.1063799999999997</v>
       </c>
       <c r="K8" s="15" t="s">
         <v>20</v>
@@ -1978,7 +1981,7 @@
       </c>
       <c r="J9" s="5">
         <f ca="1">IF(Table1[[#This Row],[Price (USD)]],SUM(Table1[[#This Row],[Price (USD)]:[Shipping (USD)]]),SUM(Table1[[#This Row],[Shipping (AUD)]],Table1[[#This Row],[Price (AUD)]])*Exchange!$B$3)</f>
-        <v>6.5311799999999991</v>
+        <v>6.5331699999999993</v>
       </c>
       <c r="K9" s="15" t="s">
         <v>25</v>
@@ -2015,7 +2018,7 @@
       </c>
       <c r="J10" s="5">
         <f ca="1">IF(Table1[[#This Row],[Price (USD)]],SUM(Table1[[#This Row],[Price (USD)]:[Shipping (USD)]]),SUM(Table1[[#This Row],[Shipping (AUD)]],Table1[[#This Row],[Price (AUD)]])*Exchange!$B$3)</f>
-        <v>3.2163600000000003</v>
+        <v>3.2173400000000001</v>
       </c>
       <c r="K10" s="15" t="s">
         <v>29</v>
@@ -2065,7 +2068,7 @@
         <v>51</v>
       </c>
       <c r="E13" s="5">
-        <v>3.18</v>
+        <v>8.18</v>
       </c>
       <c r="F13" s="5">
         <v>0</v>
@@ -2078,74 +2081,94 @@
       </c>
       <c r="I13" s="5">
         <f>IF(Table1[[#This Row],[Price (AUD)]],SUM(Table1[[#This Row],[Shipping (AUD)]],Table1[[#This Row],[Price (AUD)]]),SUM(Table1[[#This Row],[Price (USD)]:[Shipping (USD)]])*Exchange!$B$2)</f>
-        <v>19.77</v>
+        <v>24.77</v>
       </c>
       <c r="J13" s="5">
         <f ca="1">IF(Table1[[#This Row],[Price (USD)]],SUM(Table1[[#This Row],[Price (USD)]:[Shipping (USD)]]),SUM(Table1[[#This Row],[Shipping (AUD)]],Table1[[#This Row],[Price (AUD)]])*Exchange!$B$3)</f>
-        <v>12.977027999999999</v>
+        <v>16.263981999999999</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E14" s="5">
-        <v>5.37</v>
-      </c>
-      <c r="F14" s="5">
-        <v>0</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H14" s="5">
-        <v>0</v>
-      </c>
+        <v>23.45</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
       <c r="I14" s="5">
         <f>IF(Table1[[#This Row],[Price (AUD)]],SUM(Table1[[#This Row],[Shipping (AUD)]],Table1[[#This Row],[Price (AUD)]]),SUM(Table1[[#This Row],[Price (USD)]:[Shipping (USD)]])*Exchange!$B$2)</f>
-        <v>5.37</v>
+        <v>23.45</v>
       </c>
       <c r="J14" s="5">
         <f ca="1">IF(Table1[[#This Row],[Price (USD)]],SUM(Table1[[#This Row],[Price (USD)]:[Shipping (USD)]]),SUM(Table1[[#This Row],[Shipping (AUD)]],Table1[[#This Row],[Price (AUD)]])*Exchange!$B$3)</f>
-        <v>3.5248680000000001</v>
-      </c>
-      <c r="L14" s="4"/>
+        <v>15.397269999999999</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="5">
+        <v>22.66</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0</v>
+      </c>
+      <c r="G15" s="6"/>
+      <c r="H15" s="5">
+        <v>0</v>
+      </c>
+      <c r="I15" s="5">
+        <f>IF(Table1[[#This Row],[Price (AUD)]],SUM(Table1[[#This Row],[Shipping (AUD)]],Table1[[#This Row],[Price (AUD)]]),SUM(Table1[[#This Row],[Price (USD)]:[Shipping (USD)]])*Exchange!$B$2)</f>
+        <v>22.66</v>
+      </c>
+      <c r="J15" s="5">
+        <f ca="1">IF(Table1[[#This Row],[Price (USD)]],SUM(Table1[[#This Row],[Price (USD)]:[Shipping (USD)]]),SUM(Table1[[#This Row],[Shipping (AUD)]],Table1[[#This Row],[Price (AUD)]])*Exchange!$B$3)</f>
+        <v>14.878556</v>
+      </c>
+      <c r="L15" s="4"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5">
+      <c r="E16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5">
         <f ca="1">SUM(Table1[Total (AUD)])</f>
-        <v>76.207800000000006</v>
-      </c>
-      <c r="J15" s="5">
+        <v>121.94072799999999</v>
+      </c>
+      <c r="J16" s="5">
         <f ca="1">SUM(Table1[Total (USD)])</f>
-        <v>50.033955999999996</v>
-      </c>
-      <c r="K15">
+        <v>80.076697999999993</v>
+      </c>
+      <c r="K16">
         <f>SUBTOTAL(103,Table1[Link])</f>
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B17" s="7"/>
-      <c r="C17" s="9"/>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18" s="7"/>
+      <c r="C18" s="9"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B18" s="8"/>
-      <c r="C18" s="9"/>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19" s="8"/>
+      <c r="C19" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2170,7 +2193,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2196,11 +2219,11 @@
       </c>
       <c r="B2" s="12" cm="1">
         <f t="array" aca="1" ref="B2" ca="1">_FV(A2,"Price")</f>
-        <v>1.5225</v>
+        <v>1.5221</v>
       </c>
       <c r="C2" s="13" cm="1">
         <f t="array" aca="1" ref="C2" ca="1">_FV(A2,"Last trade time",TRUE)</f>
-        <v>45852.318287037036</v>
+        <v>45852.410069444442</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2209,11 +2232,11 @@
       </c>
       <c r="B3" s="8" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">_FV(A3,"Price")</f>
-        <v>0.65639999999999998</v>
+        <v>0.65659999999999996</v>
       </c>
       <c r="C3" s="13" cm="1">
         <f t="array" aca="1" ref="C3" ca="1">_FV(A3,"Last trade time",TRUE)</f>
-        <v>45852.318287037036</v>
+        <v>45852.410069444442</v>
       </c>
       <c r="D3" s="9"/>
     </row>

</xml_diff>